<commit_message>
modification to test file
</commit_message>
<xml_diff>
--- a/SRC/diff-test.xlsx
+++ b/SRC/diff-test.xlsx
@@ -32,10 +32,10 @@
     <t>Test1</t>
   </si>
   <si>
-    <t>Test2</t>
+    <t>bbb</t>
   </si>
   <si>
-    <t>aaa</t>
+    <t>Test_2</t>
   </si>
 </sst>
 </file>
@@ -363,15 +363,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>